<commit_message>
Update email language: 'responses' not 'applications' + 7 new registrants
LANGUAGE IMPROVEMENTS:
- Change 'applications' to 'responses' (more accurate for voluntary registration)
- Change 'applicant' to 'everyone who registered'
- Update 'application status' to 'registration status'
- More welcoming tone reflecting invitation response vs competitive application

NEW REGISTRANTS (2229):
- Add 7 new email drafts for recent registrants
- Update EMAIL_DRAFTS_SUMMARY.md with extended tracking list
- All 29 personalized drafts ready for copy-paste sending

TECHNICAL:
- Regenerated all existing 22 drafts with improved language
- Created 7 new drafts (23-29) for additional registrants
- Updated input Excel file reflects growth in registration interest
</commit_message>
<xml_diff>
--- a/input/2025 - PMI Sydney Chapter Project Management Day of Service (PMDoS) 2025 Professional Registration (Responses).xlsx
+++ b/input/2025 - PMI Sydney Chapter Project Management Day of Service (PMDoS) 2025 Professional Registration (Responses).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PMI\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D013FB96-FC15-49A1-82FC-D93AA71F68F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4461207-6D80-436E-BCF2-E02C3E26688F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="323">
   <si>
     <t>Timestamp</t>
   </si>
@@ -758,6 +758,198 @@
   </si>
   <si>
     <t>Nikki Gittins</t>
+  </si>
+  <si>
+    <t>pharris3@optusnet.com.au</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Harrison</t>
+  </si>
+  <si>
+    <t>042114370</t>
+  </si>
+  <si>
+    <t>Program Manager</t>
+  </si>
+  <si>
+    <t>HOMES NSW</t>
+  </si>
+  <si>
+    <t>Software Implementation and/or Rollout</t>
+  </si>
+  <si>
+    <t>delivered technology solutions to state government, defence, BHP for over 30 years</t>
+  </si>
+  <si>
+    <t>Peter Robert Harrison</t>
+  </si>
+  <si>
+    <t>aishwarya.rajendran2012@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aishwarya </t>
+  </si>
+  <si>
+    <t>Rajendran</t>
+  </si>
+  <si>
+    <t>0451804880</t>
+  </si>
+  <si>
+    <t>Consulting Intern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optik Consultancy </t>
+  </si>
+  <si>
+    <t>linkedin.com/in/aishwarya-rajendran2012</t>
+  </si>
+  <si>
+    <t>Strategic Planning, Business Change Management or Change Related Initiatives, Fund Raising Initiatives, Problem Analysis and Solutioning, Expansion of Membership and/or Increasing Awareness and Support for NFP Organisation</t>
+  </si>
+  <si>
+    <t>Aishwarya Rajendran</t>
+  </si>
+  <si>
+    <t>carolmelo.pm@gmail.com</t>
+  </si>
+  <si>
+    <t>Carolina</t>
+  </si>
+  <si>
+    <t>Abelha Melo</t>
+  </si>
+  <si>
+    <t>0456206572</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Manager </t>
+  </si>
+  <si>
+    <t>CIP - Corporate Interior Projects</t>
+  </si>
+  <si>
+    <t>Business Change Management or Change Related Initiatives, Fund Raising Initiatives, Events Planning</t>
+  </si>
+  <si>
+    <t>Looking forward to go</t>
+  </si>
+  <si>
+    <t>Carolina Abelha Melo</t>
+  </si>
+  <si>
+    <t>ivonne.portoc@gmail.com</t>
+  </si>
+  <si>
+    <t>Ivonne</t>
+  </si>
+  <si>
+    <t>Portocarrero</t>
+  </si>
+  <si>
+    <t>0426737214</t>
+  </si>
+  <si>
+    <t>Ivonne.portoc@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telecommunications Engineer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entelso </t>
+  </si>
+  <si>
+    <t>Business Change Management or Change Related Initiatives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excellent opportunity to get a new knowledge </t>
+  </si>
+  <si>
+    <t>Ivonne P</t>
+  </si>
+  <si>
+    <t>RDA.JOHN@gmail.com</t>
+  </si>
+  <si>
+    <t>Richard</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>0411311008</t>
+  </si>
+  <si>
+    <t>rda.john@gmail.com</t>
+  </si>
+  <si>
+    <t>Telstra</t>
+  </si>
+  <si>
+    <t>Software Implementation and/or Rollout, Business Change Management or Change Related Initiatives, Problem Analysis and Solutioning</t>
+  </si>
+  <si>
+    <t>Most of my project work has been technical in nature.  My current project is to roll out a new system of work across the company.</t>
+  </si>
+  <si>
+    <t>Richard John</t>
+  </si>
+  <si>
+    <t>samehtalat@yahoo.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sameh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Megally </t>
+  </si>
+  <si>
+    <t>0421480021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost Manager </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sydney Water </t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sameh-megally-8aa66a7b?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank you </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sameh Megally </t>
+  </si>
+  <si>
+    <t>achintyah619@gmail.com</t>
+  </si>
+  <si>
+    <t>Achintya</t>
+  </si>
+  <si>
+    <t>Hrishikesh</t>
+  </si>
+  <si>
+    <t>0432540116</t>
+  </si>
+  <si>
+    <t>Project operations</t>
+  </si>
+  <si>
+    <t>reKro</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/achintya-h-10b694227/</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Achintya Hrishikesh</t>
   </si>
   <si>
     <t>Name</t>
@@ -809,7 +1001,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -821,6 +1013,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
     </font>
     <font>
       <u/>
@@ -991,10 +1189,10 @@
         <color rgb="FF442F65"/>
       </left>
       <right style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -1003,13 +1201,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -1018,13 +1216,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
         <color rgb="FF442F65"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -1035,7 +1233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1083,6 +1281,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1138,7 +1339,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses" displayName="Form_Responses" ref="A1:AD23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses" displayName="Form_Responses" ref="A1:AD30">
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Timestamp"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Email address"/>
@@ -1376,11 +1577,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD23"/>
+  <dimension ref="A1:AD30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3403,89 +3604,709 @@
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A23" s="14">
+      <c r="A23" s="9">
         <v>45922.751129837961</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="H23" s="15" t="s">
+      <c r="H23" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="K23" s="15" t="s">
+      <c r="K23" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="L23" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="M23" s="15" t="s">
+      <c r="L23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="M23" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="N23" s="15" t="s">
+      <c r="N23" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="O23" s="15" t="s">
+      <c r="O23" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="P23" s="15">
-        <v>5</v>
-      </c>
-      <c r="Q23" s="15">
-        <v>3</v>
-      </c>
-      <c r="R23" s="15">
-        <v>5</v>
-      </c>
-      <c r="S23" s="15">
-        <v>5</v>
-      </c>
-      <c r="T23" s="15">
-        <v>5</v>
-      </c>
-      <c r="U23" s="15">
-        <v>5</v>
-      </c>
-      <c r="V23" s="15">
-        <v>5</v>
-      </c>
-      <c r="W23" s="15">
-        <v>5</v>
-      </c>
-      <c r="X23" s="15">
-        <v>5</v>
-      </c>
-      <c r="Y23" s="15">
-        <v>5</v>
-      </c>
-      <c r="Z23" s="15">
-        <v>1</v>
-      </c>
-      <c r="AA23" s="15">
-        <v>5</v>
-      </c>
-      <c r="AB23" s="15">
-        <v>5</v>
-      </c>
-      <c r="AC23" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD23" s="17" t="s">
+      <c r="P23" s="10">
+        <v>5</v>
+      </c>
+      <c r="Q23" s="10">
+        <v>3</v>
+      </c>
+      <c r="R23" s="10">
+        <v>5</v>
+      </c>
+      <c r="S23" s="10">
+        <v>5</v>
+      </c>
+      <c r="T23" s="10">
+        <v>5</v>
+      </c>
+      <c r="U23" s="10">
+        <v>5</v>
+      </c>
+      <c r="V23" s="10">
+        <v>5</v>
+      </c>
+      <c r="W23" s="10">
+        <v>5</v>
+      </c>
+      <c r="X23" s="10">
+        <v>5</v>
+      </c>
+      <c r="Y23" s="10">
+        <v>5</v>
+      </c>
+      <c r="Z23" s="10">
+        <v>1</v>
+      </c>
+      <c r="AA23" s="10">
+        <v>5</v>
+      </c>
+      <c r="AB23" s="10">
+        <v>5</v>
+      </c>
+      <c r="AC23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD23" s="13" t="s">
         <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>45922.821832824076</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="J24" s="5">
+        <v>1808611</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="O24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P24" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q24" s="5">
+        <v>4</v>
+      </c>
+      <c r="R24" s="5">
+        <v>3</v>
+      </c>
+      <c r="S24" s="5">
+        <v>3</v>
+      </c>
+      <c r="T24" s="5">
+        <v>3</v>
+      </c>
+      <c r="U24" s="5">
+        <v>4</v>
+      </c>
+      <c r="V24" s="5">
+        <v>4</v>
+      </c>
+      <c r="W24" s="5">
+        <v>4</v>
+      </c>
+      <c r="X24" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y24" s="5">
+        <v>5</v>
+      </c>
+      <c r="Z24" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA24" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB24" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC24" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD24" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>45923.519872777775</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="K25" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="L25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="M25" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="N25" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="O25" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="P25" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="10">
+        <v>1</v>
+      </c>
+      <c r="R25" s="10">
+        <v>1</v>
+      </c>
+      <c r="S25" s="10">
+        <v>1</v>
+      </c>
+      <c r="T25" s="10">
+        <v>1</v>
+      </c>
+      <c r="U25" s="10">
+        <v>1</v>
+      </c>
+      <c r="V25" s="10">
+        <v>1</v>
+      </c>
+      <c r="W25" s="10">
+        <v>1</v>
+      </c>
+      <c r="X25" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="10">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="10">
+        <v>2</v>
+      </c>
+      <c r="AA25" s="10">
+        <v>2</v>
+      </c>
+      <c r="AB25" s="10">
+        <v>2</v>
+      </c>
+      <c r="AC25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD25" s="13" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>45923.532031203707</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="J26" s="5">
+        <v>5766316</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M26" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="N26" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="O26" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P26" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q26" s="5">
+        <v>5</v>
+      </c>
+      <c r="R26" s="5">
+        <v>5</v>
+      </c>
+      <c r="S26" s="5">
+        <v>5</v>
+      </c>
+      <c r="T26" s="5">
+        <v>5</v>
+      </c>
+      <c r="U26" s="5">
+        <v>3</v>
+      </c>
+      <c r="V26" s="5">
+        <v>2</v>
+      </c>
+      <c r="W26" s="5">
+        <v>2</v>
+      </c>
+      <c r="X26" s="5">
+        <v>2</v>
+      </c>
+      <c r="Y26" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA26" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD26" s="8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>45923.536737349539</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="K27" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="L27" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="M27" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="N27" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="O27" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="P27" s="10">
+        <v>3</v>
+      </c>
+      <c r="Q27" s="10">
+        <v>3</v>
+      </c>
+      <c r="R27" s="10">
+        <v>1</v>
+      </c>
+      <c r="S27" s="10">
+        <v>1</v>
+      </c>
+      <c r="T27" s="10">
+        <v>1</v>
+      </c>
+      <c r="U27" s="10">
+        <v>1</v>
+      </c>
+      <c r="V27" s="10">
+        <v>2</v>
+      </c>
+      <c r="W27" s="10">
+        <v>1</v>
+      </c>
+      <c r="X27" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="10">
+        <v>5</v>
+      </c>
+      <c r="Z27" s="10">
+        <v>5</v>
+      </c>
+      <c r="AA27" s="10">
+        <v>3</v>
+      </c>
+      <c r="AB27" s="10">
+        <v>5</v>
+      </c>
+      <c r="AC27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD27" s="13" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>45923.710665972219</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N28" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="O28" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P28" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q28" s="5">
+        <v>5</v>
+      </c>
+      <c r="R28" s="5">
+        <v>3</v>
+      </c>
+      <c r="S28" s="5">
+        <v>2</v>
+      </c>
+      <c r="T28" s="5">
+        <v>3</v>
+      </c>
+      <c r="U28" s="5">
+        <v>3</v>
+      </c>
+      <c r="V28" s="5">
+        <v>4</v>
+      </c>
+      <c r="W28" s="5">
+        <v>5</v>
+      </c>
+      <c r="X28" s="5">
+        <v>5</v>
+      </c>
+      <c r="Y28" s="5">
+        <v>5</v>
+      </c>
+      <c r="Z28" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA28" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB28" s="5">
+        <v>2</v>
+      </c>
+      <c r="AC28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD28" s="8" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
+        <v>45923.782899583333</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="J29" s="10">
+        <v>1142299</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="L29" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="M29" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="N29" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="O29" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="P29" s="10">
+        <v>5</v>
+      </c>
+      <c r="Q29" s="10">
+        <v>5</v>
+      </c>
+      <c r="R29" s="10">
+        <v>5</v>
+      </c>
+      <c r="S29" s="10">
+        <v>5</v>
+      </c>
+      <c r="T29" s="10">
+        <v>1</v>
+      </c>
+      <c r="U29" s="10">
+        <v>5</v>
+      </c>
+      <c r="V29" s="10">
+        <v>5</v>
+      </c>
+      <c r="W29" s="10">
+        <v>2</v>
+      </c>
+      <c r="X29" s="10">
+        <v>2</v>
+      </c>
+      <c r="Y29" s="10">
+        <v>5</v>
+      </c>
+      <c r="Z29" s="10">
+        <v>2</v>
+      </c>
+      <c r="AA29" s="10">
+        <v>2</v>
+      </c>
+      <c r="AB29" s="10">
+        <v>2</v>
+      </c>
+      <c r="AC29" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD29" s="13" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
+        <v>45924.576281643516</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="H30" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="I30" s="17" t="s">
+        <v>306</v>
+      </c>
+      <c r="K30" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="L30" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="M30" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="N30" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="O30" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="P30" s="15">
+        <v>4</v>
+      </c>
+      <c r="Q30" s="15">
+        <v>4</v>
+      </c>
+      <c r="R30" s="15">
+        <v>3</v>
+      </c>
+      <c r="S30" s="15">
+        <v>2</v>
+      </c>
+      <c r="T30" s="15">
+        <v>2</v>
+      </c>
+      <c r="U30" s="15">
+        <v>2</v>
+      </c>
+      <c r="V30" s="15">
+        <v>2</v>
+      </c>
+      <c r="W30" s="15">
+        <v>3</v>
+      </c>
+      <c r="X30" s="15">
+        <v>3</v>
+      </c>
+      <c r="Y30" s="15">
+        <v>2</v>
+      </c>
+      <c r="Z30" s="15">
+        <v>5</v>
+      </c>
+      <c r="AA30" s="15">
+        <v>5</v>
+      </c>
+      <c r="AB30" s="15">
+        <v>2</v>
+      </c>
+      <c r="AC30" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD30" s="18" t="s">
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -3507,10 +4328,13 @@
     <hyperlink ref="I20" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="I21" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
     <hyperlink ref="I22" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="I25" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="I29" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="I30" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId18"/>
+    <tablePart r:id="rId21"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3531,91 +4355,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>246</v>
+      <c r="A1" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>248</v>
+      <c r="A2" s="19" t="s">
+        <v>311</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>249</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>250</v>
+      <c r="A3" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>248</v>
+      <c r="A4" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>252</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>248</v>
+      <c r="A5" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>253</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>250</v>
+      <c r="A6" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>254</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>250</v>
+      <c r="A7" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>255</v>
+      <c r="B8" s="19" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>256</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>250</v>
+      <c r="A9" s="19" t="s">
+        <v>320</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>250</v>
+      <c r="A10" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>258</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>250</v>
+      <c r="A11" s="19" t="s">
+        <v>322</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>